<commit_message>
feat: add date attribute to data
</commit_message>
<xml_diff>
--- a/book data.xlsx
+++ b/book data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B089D4-5B06-4FE9-9A7F-B21652FE1E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C85440A-B89D-44B5-A9B5-0E9FF9FAEE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Ten houseguests, trapped on an isolated island, are the prey of a diabolical killer. A famous nursery rhyme is framed and hung in every room of the mansion: Ten little Indian boys went out to dine; One choked his little self and then there were nine ... When they realize that murders are occurring as described in the rhyme, terror mounts. Who has choreographed this dastardly scheme? And who will be left to tell the tale?</t>
   </si>
   <si>
-    <t>16 And Then There Were None.jpg</t>
-  </si>
-  <si>
     <t xml:space="preserve">I'll Be Gone in the Dark: One Woman's Obsessive Search for the Golden State Killer </t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>For more than ten years, a mysterious and violent predator committed fifty sexual assaults in Northern California before moving south, where he perpetrated ten sadistic murders. Then he disappeared, eluding capture by multiple police forces and some of the best detectives in the area.
 Three decades later, Michelle McNamara, a true crime journalist who created the popular website TrueCrimeDiary.com, was determined to find the violent psychopath she called "the Golden State Killer." Michelle pored over police reports, interviewed victims, and embedded herself in the online communities that were as obsessed with the case as she was.
 I'll Be Gone in the Dark--the masterpiece McNamara was writing at the time of her sudden death--offers an atmospheric snapshot of a moment in American history and a chilling account of a criminal mastermind and the wreckage he left behind. It is also a portrait of a woman's obsession and her unflagging pursuit of the truth. Utterly original and compelling, it has been hailed as a modern true crime classic--one which fulfilled Michelle's dream: helping unmask the Golden State Killer.</t>
-  </si>
-  <si>
-    <t>17 I'll Be Gone in the Dark.jpg</t>
   </si>
   <si>
     <t>The Murder of Roger Ackroyd</t>
@@ -369,13 +363,48 @@
     <t>James B. Stewart</t>
   </si>
   <si>
-    <t>27 Blind Eye.jpg</t>
-  </si>
-  <si>
     <t>A medical thriller from Pulitzer Prize-winning author James B. Stewart about serial killer doctor Michael Swango and the medical community that chose to turn a blind eye on his criminal activities.
 No one could believe that the handsome young doctor might be a serial killer. Wherever he was hired—in Ohio, Illinois, New York, South Dakota—Michael Swango at first seemed the model physician. Then his patients began dying under suspicious circumstances.
 At once a gripping read and a hard-hitting look at the inner workings of the American medical system, Blind Eye describes a professional hierarchy where doctors repeatedly accept the word of fellow physicians over that of nurses, hospital employees, and patients—even as horrible truths begin to emerge. With the prodigious investigative reporting that has defined his Pulitzer Prize-winning career, James B. Stewart has tracked down survivors, relatives of victims, and shaken coworkers to unearth the evidence that may finally lead to Swango's conviction.
 Combining meticulous research with spellbinding prose, Stewart has written a shocking chronicle of a psychopathic doctor and of the medical establishment that chose to turn a blind eye on his criminal activities.</t>
+  </si>
+  <si>
+    <t>27 Blind Eye.jpg</t>
+  </si>
+  <si>
+    <t>A Study in Scarlet</t>
+  </si>
+  <si>
+    <t>Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t>Our first meeting with Sherlock Holmes. And John Watson's too! The young doctor is astonished by Holmes' many idiosyncrasies, including his talents on the violin.
+But it's not long before Sherlock Holmes, with Watson in tow, is working with Scotland Yard investigating the murder of two Americans whose deaths have some mysterious connection to sinister groups gathering power in both Britain and America.
+Here's where it all began, 'A Study in Scarlet.' Meet Sherlock Holmes, one of the world's leading consulting detectives - fictional of course!</t>
+  </si>
+  <si>
+    <t>28 A Study in Scarlet.jpg</t>
+  </si>
+  <si>
+    <t>The Girls We Sent Away</t>
+  </si>
+  <si>
+    <t>Meagan Church</t>
+  </si>
+  <si>
+    <t>North Carolina, 1960s. Lorraine has it all-the boyfriend, the good grades, the white picket fence, the ambition to become the first woman astronaut. But when she-the darling girl-next-door-becomes pregnant, she learns that love is conditional and ambition has its limits. In an effort to hide their daughter's secret shame, her parents send her away to a maternity home-a common solution for "wayward" girls during that time period. Lorraine soon realizes that instead of being a safe haven, the home forces unwed mothers to relinquish parental rights and place their babies for adoption. Lorraine must decide if she has the agency and power to fight to keep her baby or if she must submit to the rules of the society she once admired. Set in the Baby Scoop Era, The Girls We Sent Away juxtaposes the breakthrough technologies of the Race to Space with the societal realities that kept women grounded.</t>
+  </si>
+  <si>
+    <t>29 The Girls We Sent Away.jpg</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>16 I'll Be Gone in the Dark.jpg</t>
+  </si>
+  <si>
+    <t>17 And Then There Were None.jpg</t>
   </si>
 </sst>
 </file>
@@ -411,19 +440,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{8CCB3605-5DDB-4D86-9363-829160037E6F}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{A1F954B3-F3EB-4108-BA2D-461027C8B83B}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -699,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -712,9 +742,10 @@
     <col min="3" max="3" width="28.453125" customWidth="1"/>
     <col min="4" max="4" width="255.6328125" customWidth="1"/>
     <col min="5" max="5" width="31.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,8 +761,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="101.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A4" si="0">ROW()-1</f>
         <v>1</v>
@@ -748,8 +782,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>44757</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -766,8 +803,11 @@
       <c r="E3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="174" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="3">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="174" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -784,8 +824,11 @@
       <c r="E4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="3">
+        <v>44788</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A25" si="1">ROW()-1</f>
         <v>4</v>
@@ -802,8 +845,11 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="3">
+        <v>45078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -820,8 +866,11 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="3">
+        <v>45206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -838,8 +887,11 @@
       <c r="E7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="3">
+        <v>45206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -856,8 +908,11 @@
       <c r="E8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="3">
+        <v>45217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="159.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -874,8 +929,11 @@
       <c r="E9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="3">
+        <v>45338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -892,8 +950,11 @@
       <c r="E10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="3">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -910,8 +971,11 @@
       <c r="E11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="3">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -928,8 +992,11 @@
       <c r="E12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="3">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -946,8 +1013,11 @@
       <c r="E13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="145" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F13" s="3">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="145" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -964,8 +1034,11 @@
       <c r="E14" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="3">
+        <v>45419</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -982,8 +1055,11 @@
       <c r="E15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="3">
+        <v>45419</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1000,220 +1076,299 @@
       <c r="E16" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="3">
+        <v>45419</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="3">
+        <v>45434</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>62</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="101.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1">
-        <f t="shared" si="1"/>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F18" s="3">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>67</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>69</v>
       </c>
       <c r="C19" t="s">
         <v>49</v>
       </c>
       <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="3">
+        <v>45458</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>70</v>
       </c>
-      <c r="E19" t="s">
+      <c r="C20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="F20" s="3">
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>74</v>
-      </c>
-      <c r="E20" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>76</v>
       </c>
       <c r="C21" t="s">
         <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="3">
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>77</v>
       </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="116" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="F22" s="3">
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>81</v>
-      </c>
-      <c r="E22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="72.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>83</v>
       </c>
       <c r="C23" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="3">
+        <v>45498</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="E23" t="s">
+      <c r="C24" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>86</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>87</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" s="3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>88</v>
       </c>
-      <c r="E24" t="s">
+      <c r="C25" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>90</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>91</v>
       </c>
-      <c r="D25" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="3">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <f>ROW()-1</f>
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
         <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="F26" s="3">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <f>ROW()-1</f>
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>98</v>
       </c>
-      <c r="D27" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+      <c r="F27" s="3">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" s="3">
+        <v>45541</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s">
         <v>104</v>
       </c>
-      <c r="E28" t="s">
-        <v>103</v>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="3">
+        <v>45543</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F30" s="3">
+        <v>45546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>